<commit_message>
40 new test cases
</commit_message>
<xml_diff>
--- a/Test case final.xlsx
+++ b/Test case final.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="195">
   <si>
     <t>TEST CASE NO</t>
   </si>
@@ -276,9 +276,6 @@
     <t>user should able to see the test management drop downs</t>
   </si>
   <si>
-    <t>To check the first sub item test status</t>
-  </si>
-  <si>
     <t xml:space="preserve">To check test management  in menu bar is  working correctly for auto tools page </t>
   </si>
   <si>
@@ -297,9 +294,6 @@
     <t>3.Observe the rows and columns</t>
   </si>
   <si>
-    <t>3.Table consists of 5 rows with 5 column Headers</t>
-  </si>
-  <si>
     <t xml:space="preserve">2.A page with heading test status  and table with table headers                                              - test status ID,                                               -test description,                                          -test status,                                                    -create date,                                                    - update date </t>
   </si>
   <si>
@@ -309,36 +303,12 @@
     <t>To verify the first column heading of status page</t>
   </si>
   <si>
-    <t>2.Observe the rows and columns</t>
-  </si>
-  <si>
-    <t>2..Table consists of 5 rows with 5 column Headers</t>
-  </si>
-  <si>
-    <t>3.observe the first column</t>
-  </si>
-  <si>
-    <t>3.First column header Test status ID displayed</t>
-  </si>
-  <si>
-    <t>2.Second column heading Test Description is displayed</t>
-  </si>
-  <si>
     <t>To verify the second column  heading of status page</t>
   </si>
   <si>
     <t xml:space="preserve">To verify the third column header of status page </t>
   </si>
   <si>
-    <t>2.observe the second column</t>
-  </si>
-  <si>
-    <t>2.observe the third column</t>
-  </si>
-  <si>
-    <t>2.Third column header Test status is displayed</t>
-  </si>
-  <si>
     <t>Test description column heading in bold  should display with all the data under it</t>
   </si>
   <si>
@@ -352,6 +322,288 @@
   </si>
   <si>
     <t>2. A drop down should be displayed with two items                                       -My profile                                                        -Logout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To verify the fouth column header of status page </t>
+  </si>
+  <si>
+    <t>Create date column header in bold  should display with all the data under it</t>
+  </si>
+  <si>
+    <t>Update date column header in bold should display with all the data under it</t>
+  </si>
+  <si>
+    <t>To check the first item test status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To verify the sixth column header of status page </t>
+  </si>
+  <si>
+    <t xml:space="preserve">sixth column should not have header </t>
+  </si>
+  <si>
+    <t>To verify the seventh column header of status page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">seventh column should not have header </t>
+  </si>
+  <si>
+    <t>To verify the data below the Test status header of test status page</t>
+  </si>
+  <si>
+    <t>4.observe the first column</t>
+  </si>
+  <si>
+    <t>3..Table consists of 5 rows with 5 column Headers</t>
+  </si>
+  <si>
+    <t>4.First column header Test status ID displayed</t>
+  </si>
+  <si>
+    <t>2.Table consists of 5 rows with 5 column Headers</t>
+  </si>
+  <si>
+    <t>3.observe the second column</t>
+  </si>
+  <si>
+    <t>3.Second column heading Test Description is displayed</t>
+  </si>
+  <si>
+    <t>3.observe the third column</t>
+  </si>
+  <si>
+    <t>3.Third colum n header Test status is displayed</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2.click on test management -&gt; test status</t>
+  </si>
+  <si>
+    <t>3.observe the fourth column</t>
+  </si>
+  <si>
+    <t>3.Fourth colum n header Create date displayed</t>
+  </si>
+  <si>
+    <t>2..click on test management -&gt; test status</t>
+  </si>
+  <si>
+    <t>3.observe the fifth column</t>
+  </si>
+  <si>
+    <t>3.Fifth colum n header Update date displayed</t>
+  </si>
+  <si>
+    <t>3.observe the sixth column</t>
+  </si>
+  <si>
+    <t>3.sixth column displays with no header</t>
+  </si>
+  <si>
+    <t>3.observe the seventh column</t>
+  </si>
+  <si>
+    <t>2.click on test management -&gt; test status</t>
+  </si>
+  <si>
+    <t>3. observe the first column</t>
+  </si>
+  <si>
+    <t>3..Under the Test ID's header all the test status Id's are displayed</t>
+  </si>
+  <si>
+    <t>All the Test status ID's should be displayed under test status ID Column</t>
+  </si>
+  <si>
+    <t>4.Id's 1-4  are displayed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To verify the data below the test description header of test status page </t>
+  </si>
+  <si>
+    <t>3. observe the second column</t>
+  </si>
+  <si>
+    <t>3.Under the Test description header all the test descriptions are displayed</t>
+  </si>
+  <si>
+    <t>4. First description -tests the login is diplayed</t>
+  </si>
+  <si>
+    <t>All the Test descriptions should be displayed under test description column</t>
+  </si>
+  <si>
+    <t>3. observe the third column</t>
+  </si>
+  <si>
+    <t>3.Under the test status header all the test status as running are displayed</t>
+  </si>
+  <si>
+    <t>4.First status - Running is displayed</t>
+  </si>
+  <si>
+    <t>All the Test status should be displayed under the test status column</t>
+  </si>
+  <si>
+    <t>4.first create date - 2016-01-28 15:20:03.0 is displayed</t>
+  </si>
+  <si>
+    <t>All the create dates should be displayed under the create dates column</t>
+  </si>
+  <si>
+    <t>To verify the data below the create date header of the test status page</t>
+  </si>
+  <si>
+    <t>To verify the data below the update date header of the test status page</t>
+  </si>
+  <si>
+    <t>3.Under the create date header all the test status as running are displayed</t>
+  </si>
+  <si>
+    <t>3.Under the update date header all the test status as running are displayed</t>
+  </si>
+  <si>
+    <t>4.First update date2016-10-10 11:08:05.0</t>
+  </si>
+  <si>
+    <t>All the update dates should be displayed under the create dates column</t>
+  </si>
+  <si>
+    <t>3.Under the sixth column start  buttons are displayed</t>
+  </si>
+  <si>
+    <t>All the start buttons sholud be displayed under this column</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To verify the start button is working </t>
+  </si>
+  <si>
+    <t>3.click the start button in the sixth column</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.The button should start running and display the button as running and </t>
+  </si>
+  <si>
+    <t>The button should be displayed like running in blue and the data test status  also should display running</t>
+  </si>
+  <si>
+    <t>2.click on test management -&gt; test suite status</t>
+  </si>
+  <si>
+    <t>3.Table consists of 5 rows with 7 columns</t>
+  </si>
+  <si>
+    <t>3.observe the table in the test suite status</t>
+  </si>
+  <si>
+    <t>2.A table consists of 5 rows with 7 columns</t>
+  </si>
+  <si>
+    <t>3.The table consist of 5 rows and 4 column header</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The test suite status page consists of 5 rows and 7 columns </t>
+  </si>
+  <si>
+    <t>To check the second drop down in the test management</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.observe the first column of the table </t>
+  </si>
+  <si>
+    <t>To verify the data below sixth column of the test status page</t>
+  </si>
+  <si>
+    <t>To verify the data below the  seventh column</t>
+  </si>
+  <si>
+    <t>3. under the seventh column all the latest Report hyperlinks are sidplayed</t>
+  </si>
+  <si>
+    <t>Under the seventh column it should display all the latest report link hyperlinks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to check the latest report links are  working for test status page </t>
+  </si>
+  <si>
+    <t>3. click the the latest reportLink</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.The link is navigating to another page in which it consists of two tables </t>
+  </si>
+  <si>
+    <t>The link should navigate to another page which should have header  test run report with all the details</t>
+  </si>
+  <si>
+    <t>3.observe the second column of the table</t>
+  </si>
+  <si>
+    <t>To verify the first column header of the test suite status page</t>
+  </si>
+  <si>
+    <t>3.Firt column has the header Test suite ID's</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It should diplay  the header test ID's in the table for test suite status page </t>
+  </si>
+  <si>
+    <t>To verify the second column of the table in  test suite status page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To verify the third column of the table in  test suite status page </t>
+  </si>
+  <si>
+    <t>3.observe the third column of the table</t>
+  </si>
+  <si>
+    <t>3.Second column has the header test suite name</t>
+  </si>
+  <si>
+    <t>IT should display the header Test suite name in the table for test suite status page</t>
+  </si>
+  <si>
+    <t>It should display the header Test suite status in the table for test suite status page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.Third columns has the header test suite status </t>
+  </si>
+  <si>
+    <t>To verify the fourth column of the table in the test suite status page</t>
+  </si>
+  <si>
+    <t>3.observe the fourth column of the table</t>
+  </si>
+  <si>
+    <t>3. Fourth columns has the header update date</t>
+  </si>
+  <si>
+    <t>It should display the header update date in the table for test suite status page</t>
+  </si>
+  <si>
+    <t>To verify the fifth column of the table in the test suite status page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.observe the fifth column of the table </t>
+  </si>
+  <si>
+    <t>3.Fifth column of the table has no header name</t>
+  </si>
+  <si>
+    <t>It should display with header name in the table for test suite status page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To verify the sixth column of the table in the test suite status page </t>
+  </si>
+  <si>
+    <t>3.Observe the sixth column of the table</t>
+  </si>
+  <si>
+    <t>3.Sixth column of the table has no header name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To verify the seventh column of the table in the test suite status page </t>
+  </si>
+  <si>
+    <t>3.observe the seventh column of the table</t>
   </si>
 </sst>
 </file>
@@ -399,7 +651,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -433,6 +685,27 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -739,10 +1012,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H70"/>
+  <dimension ref="A1:H162"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="G68" sqref="G68:G69"/>
+    <sheetView tabSelected="1" topLeftCell="A149" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="G159" sqref="G159:G161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -769,10 +1042,10 @@
       <c r="D1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="15"/>
+      <c r="F1" s="22"/>
       <c r="G1" s="4" t="s">
         <v>4</v>
       </c>
@@ -828,38 +1101,38 @@
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" ht="60" customHeight="1">
-      <c r="A5" s="14">
+      <c r="A5" s="21">
         <v>2</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="21" t="s">
         <v>36</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="13" t="s">
+      <c r="F5" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="20" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="14"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
+      <c r="A6" s="21"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
       <c r="E6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="2"/>
@@ -872,16 +1145,16 @@
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" ht="45" customHeight="1">
-      <c r="A8" s="14">
+      <c r="A8" s="21">
         <v>3</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="20" t="s">
         <v>35</v>
       </c>
       <c r="E8" s="6" t="s">
@@ -890,22 +1163,22 @@
       <c r="F8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="G8" s="20" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="30">
-      <c r="A9" s="14"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="13"/>
+      <c r="A9" s="21"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="20"/>
       <c r="E9" s="9" t="s">
         <v>22</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G9" s="13"/>
+      <c r="G9" s="20"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="2"/>
@@ -918,62 +1191,62 @@
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" ht="45" customHeight="1">
-      <c r="A11" s="13">
+      <c r="A11" s="20">
         <v>4</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="14" t="s">
+      <c r="C11" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="21" t="s">
         <v>34</v>
       </c>
       <c r="E11" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="F11" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" s="13" t="s">
+      <c r="F11" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="20" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="13"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
+      <c r="A12" s="20"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
       <c r="E12" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="13"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
+      <c r="A13" s="20"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
       <c r="E13" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
     </row>
     <row r="14" spans="1:8" ht="30">
-      <c r="A14" s="13"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
+      <c r="A14" s="20"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
       <c r="E14" s="9" t="s">
         <v>30</v>
       </c>
       <c r="F14" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="G14" s="13"/>
+      <c r="G14" s="20"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="2"/>
@@ -986,38 +1259,38 @@
       <c r="H15" s="2"/>
     </row>
     <row r="16" spans="1:8" ht="45">
-      <c r="A16" s="14">
+      <c r="A16" s="21">
         <v>5</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="16"/>
+      <c r="D16" s="23"/>
       <c r="E16" s="10" t="s">
         <v>73</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="G16" s="13" t="s">
+      <c r="G16" s="20" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="75">
-      <c r="A17" s="14"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="16"/>
+      <c r="A17" s="21"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="23"/>
       <c r="E17" s="10" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G17" s="13"/>
+      <c r="G17" s="20"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="2"/>
@@ -1030,38 +1303,38 @@
       <c r="H18" s="2"/>
     </row>
     <row r="19" spans="1:8" ht="45">
-      <c r="A19" s="14">
+      <c r="A19" s="21">
         <v>6</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="D19" s="14"/>
+      <c r="C19" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="21"/>
       <c r="E19" s="10" t="s">
         <v>73</v>
       </c>
       <c r="F19" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="G19" s="13" t="s">
+      <c r="G19" s="20" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="30">
-      <c r="A20" s="14"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
+      <c r="A20" s="21"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
       <c r="E20" s="10" t="s">
         <v>42</v>
       </c>
       <c r="F20" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="G20" s="13"/>
+      <c r="G20" s="20"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="2"/>
@@ -1074,38 +1347,38 @@
       <c r="H21" s="2"/>
     </row>
     <row r="22" spans="1:8" ht="45">
-      <c r="A22" s="14">
+      <c r="A22" s="21">
         <v>7</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="D22" s="16"/>
+      <c r="C22" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="23"/>
       <c r="E22" s="10" t="s">
         <v>72</v>
       </c>
       <c r="F22" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="G22" s="13" t="s">
+      <c r="G22" s="20" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="60">
-      <c r="A23" s="14"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="16"/>
+      <c r="A23" s="21"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="23"/>
       <c r="E23" s="9" t="s">
         <v>45</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="G23" s="13"/>
+        <v>100</v>
+      </c>
+      <c r="G23" s="20"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="12"/>
@@ -1118,134 +1391,134 @@
       <c r="H24" s="12"/>
     </row>
     <row r="25" spans="1:8" ht="60" customHeight="1">
-      <c r="A25" s="14">
+      <c r="A25" s="21">
         <v>8</v>
       </c>
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="D25" s="16"/>
+      <c r="C25" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" s="23"/>
       <c r="E25" s="8" t="s">
         <v>71</v>
       </c>
       <c r="F25" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="G25" s="14" t="s">
+      <c r="G25" s="21" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="14"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="16"/>
+      <c r="A26" s="21"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="23"/>
       <c r="E26" s="9" t="s">
         <v>49</v>
       </c>
       <c r="F26" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="G26" s="14"/>
+      <c r="G26" s="21"/>
     </row>
     <row r="27" spans="1:8" s="12" customFormat="1"/>
     <row r="28" spans="1:8" ht="45">
-      <c r="A28" s="14">
+      <c r="A28" s="21">
         <v>9</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="C28" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="D28" s="16"/>
+      <c r="C28" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="23"/>
       <c r="E28" s="8" t="s">
         <v>70</v>
       </c>
       <c r="F28" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="G28" s="13" t="s">
+      <c r="G28" s="20" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="14"/>
-      <c r="B29" s="13"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="16"/>
+      <c r="A29" s="21"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="23"/>
       <c r="E29" s="9" t="s">
         <v>53</v>
       </c>
       <c r="F29" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="G29" s="13"/>
+      <c r="G29" s="20"/>
     </row>
     <row r="30" spans="1:8" s="12" customFormat="1"/>
     <row r="31" spans="1:8" ht="45">
-      <c r="A31" s="13">
+      <c r="A31" s="20">
         <v>10</v>
       </c>
-      <c r="B31" s="13" t="s">
+      <c r="B31" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="C31" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D31" s="16"/>
+      <c r="C31" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" s="23"/>
       <c r="E31" s="8" t="s">
         <v>71</v>
       </c>
       <c r="F31" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G31" s="13" t="s">
+      <c r="G31" s="20" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="13"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="16"/>
+      <c r="A32" s="20"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="23"/>
       <c r="E32" s="9" t="s">
         <v>49</v>
       </c>
       <c r="F32" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="G32" s="13"/>
+      <c r="G32" s="20"/>
     </row>
     <row r="33" spans="1:7" ht="30">
-      <c r="A33" s="13"/>
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="16"/>
+      <c r="A33" s="20"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="23"/>
       <c r="E33" s="8" t="s">
         <v>57</v>
       </c>
       <c r="F33" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="G33" s="13"/>
+      <c r="G33" s="20"/>
     </row>
     <row r="34" spans="1:7" s="12" customFormat="1"/>
     <row r="35" spans="1:7" ht="45">
-      <c r="A35" s="14">
+      <c r="A35" s="21">
         <v>11</v>
       </c>
-      <c r="B35" s="13" t="s">
+      <c r="B35" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="C35" s="14" t="s">
+      <c r="C35" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="D35" s="14" t="s">
+      <c r="D35" s="21" t="s">
         <v>62</v>
       </c>
       <c r="E35" s="8" t="s">
@@ -1254,439 +1527,1635 @@
       <c r="F35" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G35" s="13" t="s">
+      <c r="G35" s="20" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:7">
-      <c r="A36" s="14"/>
-      <c r="B36" s="13"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
+      <c r="A36" s="21"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="21"/>
       <c r="E36" s="7" t="s">
         <v>49</v>
       </c>
       <c r="F36" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="G36" s="13"/>
+      <c r="G36" s="20"/>
     </row>
     <row r="37" spans="1:7" ht="45">
-      <c r="A37" s="14"/>
-      <c r="B37" s="13"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="14"/>
+      <c r="A37" s="21"/>
+      <c r="B37" s="20"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="21"/>
       <c r="E37" s="8" t="s">
         <v>63</v>
       </c>
       <c r="F37" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="G37" s="13"/>
+      <c r="G37" s="20"/>
     </row>
     <row r="38" spans="1:7" s="12" customFormat="1"/>
     <row r="39" spans="1:7" ht="45">
-      <c r="A39" s="14">
+      <c r="A39" s="21">
         <v>12</v>
       </c>
-      <c r="B39" s="13" t="s">
+      <c r="B39" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="C39" s="14" t="s">
+      <c r="C39" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="D39" s="16"/>
+      <c r="D39" s="23"/>
       <c r="E39" s="8" t="s">
         <v>72</v>
       </c>
       <c r="F39" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G39" s="13" t="s">
+      <c r="G39" s="20" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="14"/>
-      <c r="B40" s="13"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="16"/>
+      <c r="A40" s="21"/>
+      <c r="B40" s="20"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="23"/>
       <c r="E40" s="10" t="s">
         <v>49</v>
       </c>
       <c r="F40" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="G40" s="13"/>
+      <c r="G40" s="20"/>
     </row>
     <row r="41" spans="1:7" ht="150">
-      <c r="A41" s="14"/>
-      <c r="B41" s="13"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="16"/>
+      <c r="A41" s="21"/>
+      <c r="B41" s="20"/>
+      <c r="C41" s="21"/>
+      <c r="D41" s="23"/>
       <c r="E41" s="8" t="s">
         <v>67</v>
       </c>
       <c r="F41" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="G41" s="13"/>
+      <c r="G41" s="20"/>
     </row>
     <row r="42" spans="1:7" s="12" customFormat="1"/>
     <row r="43" spans="1:7" ht="45">
-      <c r="A43" s="13">
+      <c r="A43" s="20">
         <v>13</v>
       </c>
-      <c r="B43" s="13" t="s">
+      <c r="B43" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="C43" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="D43" s="14"/>
+      <c r="C43" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D43" s="21"/>
       <c r="E43" s="8" t="s">
         <v>72</v>
       </c>
       <c r="F43" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G43" s="13" t="s">
+      <c r="G43" s="20" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="13"/>
-      <c r="B44" s="13"/>
-      <c r="C44" s="14"/>
-      <c r="D44" s="14"/>
+      <c r="A44" s="20"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="21"/>
+      <c r="D44" s="21"/>
       <c r="E44" s="8" t="s">
         <v>49</v>
       </c>
       <c r="F44" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="G44" s="13"/>
+      <c r="G44" s="20"/>
     </row>
     <row r="45" spans="1:7" ht="30">
-      <c r="A45" s="13"/>
-      <c r="B45" s="13"/>
-      <c r="C45" s="14"/>
-      <c r="D45" s="14"/>
+      <c r="A45" s="20"/>
+      <c r="B45" s="20"/>
+      <c r="C45" s="21"/>
+      <c r="D45" s="21"/>
       <c r="E45" s="8" t="s">
         <v>74</v>
       </c>
       <c r="F45" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="G45" s="13"/>
+      <c r="G45" s="20"/>
     </row>
     <row r="46" spans="1:7" s="12" customFormat="1"/>
     <row r="47" spans="1:7" ht="60" customHeight="1">
-      <c r="A47" s="14">
+      <c r="A47" s="21">
         <v>14</v>
       </c>
-      <c r="B47" s="13" t="s">
+      <c r="B47" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="C47" s="14" t="s">
+      <c r="C47" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="D47" s="14"/>
+      <c r="D47" s="21"/>
       <c r="E47" s="8" t="s">
         <v>72</v>
       </c>
       <c r="F47" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G47" s="13" t="s">
+      <c r="G47" s="20" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="48" spans="1:7">
-      <c r="A48" s="14"/>
-      <c r="B48" s="13"/>
-      <c r="C48" s="14"/>
-      <c r="D48" s="14"/>
+      <c r="A48" s="21"/>
+      <c r="B48" s="20"/>
+      <c r="C48" s="21"/>
+      <c r="D48" s="21"/>
       <c r="E48" s="7" t="s">
         <v>49</v>
       </c>
       <c r="F48" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="G48" s="13"/>
+      <c r="G48" s="20"/>
     </row>
     <row r="49" spans="1:7" ht="30">
-      <c r="A49" s="14"/>
-      <c r="B49" s="13"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
+      <c r="A49" s="21"/>
+      <c r="B49" s="20"/>
+      <c r="C49" s="21"/>
+      <c r="D49" s="21"/>
       <c r="E49" s="8" t="s">
         <v>79</v>
       </c>
       <c r="F49" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="G49" s="13"/>
+      <c r="G49" s="20"/>
     </row>
     <row r="50" spans="1:7" s="12" customFormat="1"/>
     <row r="51" spans="1:7" ht="75" customHeight="1">
-      <c r="A51" s="14">
+      <c r="A51" s="21">
         <v>15</v>
       </c>
-      <c r="B51" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="C51" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="D51" s="16"/>
+      <c r="B51" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="C51" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D51" s="23"/>
       <c r="E51" s="8" t="s">
         <v>72</v>
       </c>
       <c r="F51" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G51" s="13" t="s">
+      <c r="G51" s="20" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="30">
-      <c r="A52" s="14"/>
-      <c r="B52" s="13"/>
-      <c r="C52" s="14"/>
-      <c r="D52" s="16"/>
+      <c r="A52" s="21"/>
+      <c r="B52" s="20"/>
+      <c r="C52" s="21"/>
+      <c r="D52" s="23"/>
       <c r="E52" s="8" t="s">
         <v>82</v>
       </c>
       <c r="F52" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="G52" s="13"/>
+      <c r="G52" s="20"/>
     </row>
     <row r="53" spans="1:7" s="12" customFormat="1"/>
     <row r="54" spans="1:7" ht="45">
-      <c r="A54" s="13">
-        <v>16</v>
-      </c>
-      <c r="B54" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="C54" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="D54" s="16"/>
+      <c r="A54" s="20">
+        <v>16</v>
+      </c>
+      <c r="B54" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="C54" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D54" s="23"/>
       <c r="E54" s="8" t="s">
         <v>72</v>
       </c>
       <c r="F54" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G54" s="13" t="s">
-        <v>89</v>
+      <c r="G54" s="20" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="90">
-      <c r="A55" s="13"/>
-      <c r="B55" s="13"/>
-      <c r="C55" s="14"/>
-      <c r="D55" s="16"/>
+      <c r="A55" s="20"/>
+      <c r="B55" s="20"/>
+      <c r="C55" s="21"/>
+      <c r="D55" s="23"/>
       <c r="E55" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="F55" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="F55" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="G55" s="13"/>
+      <c r="G55" s="20"/>
     </row>
     <row r="56" spans="1:7" s="12" customFormat="1"/>
     <row r="57" spans="1:7" ht="45">
-      <c r="A57" s="13">
+      <c r="A57" s="20">
         <v>17</v>
       </c>
-      <c r="B57" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="C57" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D57" s="16"/>
+      <c r="B57" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="C57" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D57" s="23"/>
       <c r="E57" s="8" t="s">
         <v>72</v>
       </c>
       <c r="F57" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G57" s="13" t="s">
-        <v>94</v>
+      <c r="G57" s="20" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="105">
-      <c r="A58" s="13"/>
-      <c r="B58" s="13"/>
-      <c r="C58" s="13"/>
-      <c r="D58" s="16"/>
-      <c r="E58" s="8" t="s">
-        <v>87</v>
+      <c r="A58" s="20"/>
+      <c r="B58" s="20"/>
+      <c r="C58" s="20"/>
+      <c r="D58" s="23"/>
+      <c r="E58" s="13" t="s">
+        <v>86</v>
       </c>
       <c r="F58" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="G58" s="13"/>
+        <v>91</v>
+      </c>
+      <c r="G58" s="20"/>
     </row>
     <row r="59" spans="1:7" ht="30">
-      <c r="A59" s="13"/>
-      <c r="B59" s="13"/>
-      <c r="C59" s="13"/>
-      <c r="D59" s="16"/>
+      <c r="A59" s="20"/>
+      <c r="B59" s="20"/>
+      <c r="C59" s="20"/>
+      <c r="D59" s="23"/>
       <c r="E59" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="F59" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="G59" s="13"/>
+        <v>90</v>
+      </c>
+      <c r="F59" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="G59" s="20"/>
     </row>
     <row r="60" spans="1:7" s="12" customFormat="1"/>
     <row r="61" spans="1:7" ht="45">
-      <c r="A61" s="14">
+      <c r="A61" s="21">
         <v>18</v>
       </c>
-      <c r="B61" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="C61" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="D61" s="16"/>
+      <c r="B61" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="C61" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D61" s="23"/>
       <c r="E61" s="8" t="s">
         <v>72</v>
       </c>
       <c r="F61" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G61" s="13" t="s">
+      <c r="G61" s="20" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="30">
+      <c r="A62" s="21"/>
+      <c r="B62" s="20"/>
+      <c r="C62" s="21"/>
+      <c r="D62" s="23"/>
+      <c r="E62" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F62" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="G62" s="20"/>
+    </row>
+    <row r="63" spans="1:7" ht="30">
+      <c r="A63" s="21"/>
+      <c r="B63" s="20"/>
+      <c r="C63" s="21"/>
+      <c r="D63" s="23"/>
+      <c r="E63" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="F63" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="G63" s="20"/>
+    </row>
+    <row r="64" spans="1:7" ht="30">
+      <c r="A64" s="21"/>
+      <c r="B64" s="20"/>
+      <c r="C64" s="21"/>
+      <c r="D64" s="23"/>
+      <c r="E64" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="F64" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="G64" s="20"/>
+    </row>
+    <row r="65" spans="1:7" s="12" customFormat="1"/>
+    <row r="66" spans="1:7" ht="45">
+      <c r="A66" s="20">
+        <v>19</v>
+      </c>
+      <c r="B66" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="C66" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D66" s="23"/>
+      <c r="E66" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="F66" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G66" s="20" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="30">
+      <c r="A67" s="20"/>
+      <c r="B67" s="20"/>
+      <c r="C67" s="21"/>
+      <c r="D67" s="23"/>
+      <c r="E67" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F67" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="G67" s="20"/>
+    </row>
+    <row r="68" spans="1:7" ht="30">
+      <c r="A68" s="20"/>
+      <c r="B68" s="20"/>
+      <c r="C68" s="21"/>
+      <c r="D68" s="23"/>
+      <c r="E68" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="F68" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="G68" s="20"/>
+    </row>
+    <row r="69" spans="1:7" s="12" customFormat="1"/>
+    <row r="70" spans="1:7" ht="45">
+      <c r="A70" s="21">
+        <v>20</v>
+      </c>
+      <c r="B70" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="C70" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D70" s="23"/>
+      <c r="E70" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F70" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G70" s="20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="30">
+      <c r="A71" s="21"/>
+      <c r="B71" s="20"/>
+      <c r="C71" s="21"/>
+      <c r="D71" s="23"/>
+      <c r="E71" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F71" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="G71" s="20"/>
+    </row>
+    <row r="72" spans="1:7" ht="30">
+      <c r="A72" s="21"/>
+      <c r="B72" s="20"/>
+      <c r="C72" s="21"/>
+      <c r="D72" s="23"/>
+      <c r="E72" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="F72" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="G72" s="20"/>
+    </row>
+    <row r="73" spans="1:7" s="12" customFormat="1"/>
+    <row r="74" spans="1:7" ht="45">
+      <c r="A74" s="21">
+        <v>21</v>
+      </c>
+      <c r="B74" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="C74" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D74" s="23"/>
+      <c r="E74" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="F74" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G74" s="20" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="30">
+      <c r="A75" s="21"/>
+      <c r="B75" s="20"/>
+      <c r="C75" s="21"/>
+      <c r="D75" s="23"/>
+      <c r="E75" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="F75" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="G75" s="20"/>
+    </row>
+    <row r="76" spans="1:7" ht="30">
+      <c r="A76" s="21"/>
+      <c r="B76" s="20"/>
+      <c r="C76" s="21"/>
+      <c r="D76" s="23"/>
+      <c r="E76" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="F76" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="G76" s="20"/>
+    </row>
+    <row r="77" spans="1:7" s="12" customFormat="1"/>
+    <row r="78" spans="1:7" ht="45">
+      <c r="A78" s="21">
+        <v>22</v>
+      </c>
+      <c r="B78" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="C78" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D78" s="23"/>
+      <c r="E78" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="F78" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G78" s="20" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="30">
+      <c r="A79" s="21"/>
+      <c r="B79" s="20"/>
+      <c r="C79" s="21"/>
+      <c r="D79" s="23"/>
+      <c r="E79" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="F79" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="G79" s="20"/>
+    </row>
+    <row r="80" spans="1:7" ht="30">
+      <c r="A80" s="21"/>
+      <c r="B80" s="20"/>
+      <c r="C80" s="21"/>
+      <c r="D80" s="23"/>
+      <c r="E80" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="F80" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="G80" s="20"/>
+    </row>
+    <row r="81" spans="1:7" s="12" customFormat="1"/>
+    <row r="82" spans="1:7" ht="45">
+      <c r="A82" s="21">
+        <v>23</v>
+      </c>
+      <c r="B82" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="C82" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D82" s="23"/>
+      <c r="E82" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="F82" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G82" s="20" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="30">
+      <c r="A83" s="21"/>
+      <c r="B83" s="20"/>
+      <c r="C83" s="21"/>
+      <c r="D83" s="23"/>
+      <c r="E83" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="F83" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="G83" s="20"/>
+    </row>
+    <row r="84" spans="1:7" ht="30">
+      <c r="A84" s="21"/>
+      <c r="B84" s="20"/>
+      <c r="C84" s="21"/>
+      <c r="D84" s="23"/>
+      <c r="E84" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="F84" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="G84" s="20"/>
+    </row>
+    <row r="85" spans="1:7" s="12" customFormat="1"/>
+    <row r="86" spans="1:7" ht="45">
+      <c r="A86" s="21">
+        <v>24</v>
+      </c>
+      <c r="B86" s="20" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" ht="30">
-      <c r="A62" s="14"/>
-      <c r="B62" s="13"/>
-      <c r="C62" s="14"/>
-      <c r="D62" s="16"/>
-      <c r="E62" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="F62" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="G62" s="13"/>
-    </row>
-    <row r="63" spans="1:7" ht="30">
-      <c r="A63" s="14"/>
-      <c r="B63" s="13"/>
-      <c r="C63" s="14"/>
-      <c r="D63" s="16"/>
-      <c r="E63" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="F63" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="G63" s="13"/>
-    </row>
-    <row r="64" spans="1:7" s="12" customFormat="1"/>
-    <row r="65" spans="1:7" ht="45">
-      <c r="A65" s="13">
-        <v>19</v>
-      </c>
-      <c r="B65" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="C65" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="D65" s="16"/>
-      <c r="E65" s="8" t="s">
+      <c r="C86" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D86" s="23"/>
+      <c r="E86" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="F65" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G65" s="13" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" ht="30">
-      <c r="A66" s="13"/>
-      <c r="B66" s="13"/>
-      <c r="C66" s="14"/>
-      <c r="D66" s="16"/>
-      <c r="E66" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="F66" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="G66" s="13"/>
-    </row>
-    <row r="67" spans="1:7" s="12" customFormat="1"/>
-    <row r="68" spans="1:7" ht="45">
-      <c r="A68" s="14">
-        <v>20</v>
-      </c>
-      <c r="B68" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="C68" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="D68" s="16"/>
-      <c r="E68" s="8" t="s">
+      <c r="F86" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G86" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="30">
+      <c r="A87" s="21"/>
+      <c r="B87" s="20"/>
+      <c r="C87" s="20"/>
+      <c r="D87" s="23"/>
+      <c r="E87" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="F87" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="G87" s="20"/>
+    </row>
+    <row r="88" spans="1:7" ht="30">
+      <c r="A88" s="21"/>
+      <c r="B88" s="20"/>
+      <c r="C88" s="20"/>
+      <c r="D88" s="23"/>
+      <c r="E88" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="F88" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="G88" s="20"/>
+    </row>
+    <row r="89" spans="1:7" s="12" customFormat="1"/>
+    <row r="90" spans="1:7" ht="60" customHeight="1">
+      <c r="A90" s="21">
+        <v>25</v>
+      </c>
+      <c r="B90" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="C90" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D90" s="23"/>
+      <c r="E90" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="F68" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G68" s="13" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" ht="30">
-      <c r="A69" s="14"/>
-      <c r="B69" s="13"/>
-      <c r="C69" s="14"/>
-      <c r="D69" s="16"/>
-      <c r="E69" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="F69" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="G69" s="13"/>
-    </row>
-    <row r="70" spans="1:7" s="12" customFormat="1"/>
+      <c r="F90" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G90" s="20" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" ht="30">
+      <c r="A91" s="21"/>
+      <c r="B91" s="20"/>
+      <c r="C91" s="21"/>
+      <c r="D91" s="23"/>
+      <c r="E91" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="F91" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="G91" s="20"/>
+    </row>
+    <row r="92" spans="1:7" ht="30">
+      <c r="A92" s="21"/>
+      <c r="B92" s="20"/>
+      <c r="C92" s="21"/>
+      <c r="D92" s="23"/>
+      <c r="E92" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="F92" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="G92" s="20"/>
+    </row>
+    <row r="93" spans="1:7">
+      <c r="A93" s="21"/>
+      <c r="B93" s="20"/>
+      <c r="C93" s="21"/>
+      <c r="D93" s="23"/>
+      <c r="E93" s="20"/>
+      <c r="F93" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="G93" s="20"/>
+    </row>
+    <row r="94" spans="1:7" s="12" customFormat="1"/>
+    <row r="95" spans="1:7" ht="60" customHeight="1">
+      <c r="A95" s="21">
+        <v>26</v>
+      </c>
+      <c r="B95" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="C95" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D95" s="23"/>
+      <c r="E95" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="F95" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G95" s="20" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" ht="30">
+      <c r="A96" s="21"/>
+      <c r="B96" s="20"/>
+      <c r="C96" s="21"/>
+      <c r="D96" s="23"/>
+      <c r="E96" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="F96" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="G96" s="20"/>
+    </row>
+    <row r="97" spans="1:7" ht="30">
+      <c r="A97" s="21"/>
+      <c r="B97" s="20"/>
+      <c r="C97" s="21"/>
+      <c r="D97" s="23"/>
+      <c r="E97" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="F97" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="G97" s="20"/>
+    </row>
+    <row r="98" spans="1:7" ht="30">
+      <c r="A98" s="21"/>
+      <c r="B98" s="20"/>
+      <c r="C98" s="21"/>
+      <c r="D98" s="23"/>
+      <c r="E98" s="20"/>
+      <c r="F98" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="G98" s="20"/>
+    </row>
+    <row r="99" spans="1:7" s="12" customFormat="1"/>
+    <row r="100" spans="1:7" ht="60" customHeight="1">
+      <c r="A100" s="21">
+        <v>27</v>
+      </c>
+      <c r="B100" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="C100" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D100" s="23"/>
+      <c r="E100" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="F100" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G100" s="20" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" ht="30">
+      <c r="A101" s="21"/>
+      <c r="B101" s="20"/>
+      <c r="C101" s="20"/>
+      <c r="D101" s="23"/>
+      <c r="E101" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="F101" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="G101" s="20"/>
+    </row>
+    <row r="102" spans="1:7" ht="45">
+      <c r="A102" s="21"/>
+      <c r="B102" s="20"/>
+      <c r="C102" s="20"/>
+      <c r="D102" s="23"/>
+      <c r="E102" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="F102" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="G102" s="20"/>
+    </row>
+    <row r="103" spans="1:7">
+      <c r="A103" s="21"/>
+      <c r="B103" s="20"/>
+      <c r="C103" s="20"/>
+      <c r="D103" s="23"/>
+      <c r="E103" s="20"/>
+      <c r="F103" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="G103" s="20"/>
+    </row>
+    <row r="104" spans="1:7" s="12" customFormat="1"/>
+    <row r="105" spans="1:7" ht="60" customHeight="1">
+      <c r="A105" s="21">
+        <v>28</v>
+      </c>
+      <c r="B105" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="C105" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D105" s="21"/>
+      <c r="E105" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="F105" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G105" s="20" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" ht="30">
+      <c r="A106" s="21"/>
+      <c r="B106" s="20"/>
+      <c r="C106" s="21"/>
+      <c r="D106" s="21"/>
+      <c r="E106" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="F106" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="G106" s="20"/>
+    </row>
+    <row r="107" spans="1:7" ht="45">
+      <c r="A107" s="21"/>
+      <c r="B107" s="20"/>
+      <c r="C107" s="21"/>
+      <c r="D107" s="21"/>
+      <c r="E107" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="F107" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="G107" s="20"/>
+    </row>
+    <row r="108" spans="1:7" ht="30">
+      <c r="A108" s="21"/>
+      <c r="B108" s="20"/>
+      <c r="C108" s="21"/>
+      <c r="D108" s="21"/>
+      <c r="E108" s="20"/>
+      <c r="F108" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="G108" s="20"/>
+    </row>
+    <row r="109" spans="1:7" s="12" customFormat="1"/>
+    <row r="110" spans="1:7" ht="60" customHeight="1">
+      <c r="A110" s="21">
+        <v>29</v>
+      </c>
+      <c r="B110" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="C110" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D110" s="23"/>
+      <c r="E110" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="F110" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G110" s="20" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" ht="30">
+      <c r="A111" s="21"/>
+      <c r="B111" s="20"/>
+      <c r="C111" s="21"/>
+      <c r="D111" s="23"/>
+      <c r="E111" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="F111" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="G111" s="20"/>
+    </row>
+    <row r="112" spans="1:7" ht="45">
+      <c r="A112" s="21"/>
+      <c r="B112" s="20"/>
+      <c r="C112" s="21"/>
+      <c r="D112" s="23"/>
+      <c r="E112" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="F112" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="G112" s="20"/>
+    </row>
+    <row r="113" spans="1:7" ht="30">
+      <c r="A113" s="21"/>
+      <c r="B113" s="20"/>
+      <c r="C113" s="21"/>
+      <c r="D113" s="23"/>
+      <c r="E113" s="20"/>
+      <c r="F113" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="G113" s="20"/>
+    </row>
+    <row r="114" spans="1:7" s="12" customFormat="1"/>
+    <row r="115" spans="1:7" ht="45">
+      <c r="A115" s="21">
+        <v>30</v>
+      </c>
+      <c r="B115" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="C115" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D115" s="21"/>
+      <c r="E115" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="F115" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="G115" s="20" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" ht="30">
+      <c r="A116" s="21"/>
+      <c r="B116" s="20"/>
+      <c r="C116" s="21"/>
+      <c r="D116" s="21"/>
+      <c r="E116" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="F116" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="G116" s="20"/>
+    </row>
+    <row r="117" spans="1:7" ht="30">
+      <c r="A117" s="21"/>
+      <c r="B117" s="20"/>
+      <c r="C117" s="21"/>
+      <c r="D117" s="21"/>
+      <c r="E117" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="F117" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="G117" s="20"/>
+    </row>
+    <row r="118" spans="1:7" s="12" customFormat="1"/>
+    <row r="119" spans="1:7" ht="45">
+      <c r="A119" s="21">
+        <v>31</v>
+      </c>
+      <c r="B119" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="C119" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D119" s="23"/>
+      <c r="E119" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="F119" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G119" s="20" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" ht="30">
+      <c r="A120" s="21"/>
+      <c r="B120" s="20"/>
+      <c r="C120" s="21"/>
+      <c r="D120" s="23"/>
+      <c r="E120" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="F120" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="G120" s="20"/>
+    </row>
+    <row r="121" spans="1:7" ht="45">
+      <c r="A121" s="21"/>
+      <c r="B121" s="20"/>
+      <c r="C121" s="21"/>
+      <c r="D121" s="23"/>
+      <c r="E121" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="F121" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="G121" s="20"/>
+    </row>
+    <row r="122" spans="1:7" s="12" customFormat="1"/>
+    <row r="123" spans="1:7" ht="45">
+      <c r="A123" s="20">
+        <v>32</v>
+      </c>
+      <c r="B123" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="C123" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D123" s="21"/>
+      <c r="E123" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="F123" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G123" s="20" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" ht="30">
+      <c r="A124" s="20"/>
+      <c r="B124" s="20"/>
+      <c r="C124" s="21"/>
+      <c r="D124" s="21"/>
+      <c r="E124" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="F124" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="G124" s="20"/>
+    </row>
+    <row r="125" spans="1:7" ht="45">
+      <c r="A125" s="20"/>
+      <c r="B125" s="20"/>
+      <c r="C125" s="21"/>
+      <c r="D125" s="21"/>
+      <c r="E125" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="F125" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="G125" s="20"/>
+    </row>
+    <row r="126" spans="1:7" s="12" customFormat="1"/>
+    <row r="127" spans="1:7" ht="60" customHeight="1">
+      <c r="A127" s="21">
+        <v>33</v>
+      </c>
+      <c r="B127" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="C127" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D127" s="23"/>
+      <c r="E127" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="F127" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G127" s="20" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" ht="30">
+      <c r="A128" s="21"/>
+      <c r="B128" s="20"/>
+      <c r="C128" s="21"/>
+      <c r="D128" s="23"/>
+      <c r="E128" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="F128" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="G128" s="20"/>
+    </row>
+    <row r="129" spans="1:7" ht="45">
+      <c r="A129" s="21"/>
+      <c r="B129" s="20"/>
+      <c r="C129" s="21"/>
+      <c r="D129" s="23"/>
+      <c r="E129" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="F129" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="G129" s="20"/>
+    </row>
+    <row r="130" spans="1:7" s="12" customFormat="1"/>
+    <row r="131" spans="1:7" ht="45">
+      <c r="A131" s="21">
+        <v>34</v>
+      </c>
+      <c r="B131" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="C131" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D131" s="21"/>
+      <c r="E131" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="F131" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G131" s="20" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" ht="30">
+      <c r="A132" s="21"/>
+      <c r="B132" s="20"/>
+      <c r="C132" s="21"/>
+      <c r="D132" s="21"/>
+      <c r="E132" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="F132" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="G132" s="20"/>
+    </row>
+    <row r="133" spans="1:7" ht="30">
+      <c r="A133" s="21"/>
+      <c r="B133" s="20"/>
+      <c r="C133" s="21"/>
+      <c r="D133" s="21"/>
+      <c r="E133" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="F133" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="G133" s="20"/>
+    </row>
+    <row r="134" spans="1:7" s="12" customFormat="1"/>
+    <row r="135" spans="1:7" ht="45">
+      <c r="A135" s="21">
+        <v>35</v>
+      </c>
+      <c r="B135" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="C135" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D135" s="23"/>
+      <c r="E135" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="F135" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G135" s="20" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" ht="30">
+      <c r="A136" s="21"/>
+      <c r="B136" s="20"/>
+      <c r="C136" s="21"/>
+      <c r="D136" s="23"/>
+      <c r="E136" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="F136" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="G136" s="20"/>
+    </row>
+    <row r="137" spans="1:7" ht="30">
+      <c r="A137" s="21"/>
+      <c r="B137" s="20"/>
+      <c r="C137" s="21"/>
+      <c r="D137" s="23"/>
+      <c r="E137" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="F137" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="G137" s="20"/>
+    </row>
+    <row r="138" spans="1:7" s="12" customFormat="1"/>
+    <row r="139" spans="1:7" ht="45">
+      <c r="A139" s="21">
+        <v>36</v>
+      </c>
+      <c r="B139" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="C139" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D139" s="23"/>
+      <c r="E139" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="F139" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G139" s="20" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" ht="30">
+      <c r="A140" s="21"/>
+      <c r="B140" s="20"/>
+      <c r="C140" s="21"/>
+      <c r="D140" s="23"/>
+      <c r="E140" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="F140" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="G140" s="20"/>
+    </row>
+    <row r="141" spans="1:7" ht="30">
+      <c r="A141" s="21"/>
+      <c r="B141" s="20"/>
+      <c r="C141" s="21"/>
+      <c r="D141" s="23"/>
+      <c r="E141" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="F141" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="G141" s="20"/>
+    </row>
+    <row r="142" spans="1:7" s="12" customFormat="1"/>
+    <row r="143" spans="1:7" ht="45">
+      <c r="A143" s="21">
+        <v>37</v>
+      </c>
+      <c r="B143" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="C143" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D143" s="23"/>
+      <c r="E143" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="F143" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G143" s="20" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" ht="30">
+      <c r="A144" s="21"/>
+      <c r="B144" s="20"/>
+      <c r="C144" s="21"/>
+      <c r="D144" s="23"/>
+      <c r="E144" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="F144" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="G144" s="20"/>
+    </row>
+    <row r="145" spans="1:7" ht="30">
+      <c r="A145" s="21"/>
+      <c r="B145" s="20"/>
+      <c r="C145" s="21"/>
+      <c r="D145" s="23"/>
+      <c r="E145" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="F145" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="G145" s="20"/>
+    </row>
+    <row r="146" spans="1:7" s="12" customFormat="1"/>
+    <row r="147" spans="1:7" ht="60" customHeight="1">
+      <c r="A147" s="21">
+        <v>38</v>
+      </c>
+      <c r="B147" s="20" t="s">
+        <v>182</v>
+      </c>
+      <c r="C147" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D147" s="23"/>
+      <c r="E147" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="F147" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G147" s="20" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" ht="30">
+      <c r="A148" s="21"/>
+      <c r="B148" s="20"/>
+      <c r="C148" s="21"/>
+      <c r="D148" s="23"/>
+      <c r="E148" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="F148" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="G148" s="20"/>
+    </row>
+    <row r="149" spans="1:7" ht="30">
+      <c r="A149" s="21"/>
+      <c r="B149" s="20"/>
+      <c r="C149" s="21"/>
+      <c r="D149" s="23"/>
+      <c r="E149" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="F149" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="G149" s="20"/>
+    </row>
+    <row r="150" spans="1:7" s="12" customFormat="1"/>
+    <row r="151" spans="1:7" ht="60" customHeight="1">
+      <c r="A151" s="21">
+        <v>39</v>
+      </c>
+      <c r="B151" s="20" t="s">
+        <v>186</v>
+      </c>
+      <c r="C151" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D151" s="23"/>
+      <c r="E151" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="F151" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G151" s="20" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" ht="30">
+      <c r="A152" s="21"/>
+      <c r="B152" s="20"/>
+      <c r="C152" s="21"/>
+      <c r="D152" s="23"/>
+      <c r="E152" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="F152" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="G152" s="20"/>
+    </row>
+    <row r="153" spans="1:7" ht="30">
+      <c r="A153" s="21"/>
+      <c r="B153" s="20"/>
+      <c r="C153" s="21"/>
+      <c r="D153" s="23"/>
+      <c r="E153" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="F153" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="G153" s="20"/>
+    </row>
+    <row r="154" spans="1:7" s="12" customFormat="1"/>
+    <row r="155" spans="1:7" ht="60" customHeight="1">
+      <c r="A155" s="21">
+        <v>40</v>
+      </c>
+      <c r="B155" s="20" t="s">
+        <v>190</v>
+      </c>
+      <c r="C155" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D155" s="23"/>
+      <c r="E155" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="F155" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G155" s="20" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" ht="30">
+      <c r="A156" s="21"/>
+      <c r="B156" s="20"/>
+      <c r="C156" s="21"/>
+      <c r="D156" s="23"/>
+      <c r="E156" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="F156" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="G156" s="20"/>
+    </row>
+    <row r="157" spans="1:7" ht="30">
+      <c r="A157" s="21"/>
+      <c r="B157" s="20"/>
+      <c r="C157" s="21"/>
+      <c r="D157" s="23"/>
+      <c r="E157" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="F157" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="G157" s="20"/>
+    </row>
+    <row r="158" spans="1:7" s="12" customFormat="1"/>
+    <row r="159" spans="1:7" ht="60" customHeight="1">
+      <c r="A159" s="21">
+        <v>41</v>
+      </c>
+      <c r="B159" s="20" t="s">
+        <v>193</v>
+      </c>
+      <c r="C159" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D159" s="23"/>
+      <c r="E159" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="F159" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G159" s="20" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" ht="30">
+      <c r="A160" s="21"/>
+      <c r="B160" s="20"/>
+      <c r="C160" s="21"/>
+      <c r="D160" s="23"/>
+      <c r="E160" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="F160" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="G160" s="20"/>
+    </row>
+    <row r="161" spans="1:7" ht="30">
+      <c r="A161" s="21"/>
+      <c r="B161" s="20"/>
+      <c r="C161" s="21"/>
+      <c r="D161" s="23"/>
+      <c r="E161" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="F161" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="G161" s="20"/>
+    </row>
+    <row r="162" spans="1:7" s="12" customFormat="1"/>
   </sheetData>
-  <mergeCells count="98">
-    <mergeCell ref="A68:A69"/>
-    <mergeCell ref="B68:B69"/>
-    <mergeCell ref="C68:C69"/>
-    <mergeCell ref="D68:D69"/>
-    <mergeCell ref="B61:B63"/>
-    <mergeCell ref="A61:A63"/>
-    <mergeCell ref="C61:C63"/>
-    <mergeCell ref="D61:D63"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="B65:B66"/>
-    <mergeCell ref="C65:C66"/>
-    <mergeCell ref="D65:D66"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="D54:D55"/>
+  <mergeCells count="208">
+    <mergeCell ref="A151:A153"/>
+    <mergeCell ref="B151:B153"/>
+    <mergeCell ref="C151:C153"/>
+    <mergeCell ref="D151:D153"/>
+    <mergeCell ref="A155:A157"/>
+    <mergeCell ref="B155:B157"/>
+    <mergeCell ref="C155:C157"/>
+    <mergeCell ref="D155:D157"/>
+    <mergeCell ref="A159:A161"/>
+    <mergeCell ref="B159:B161"/>
+    <mergeCell ref="C159:C161"/>
+    <mergeCell ref="D159:D161"/>
+    <mergeCell ref="B139:B141"/>
+    <mergeCell ref="A139:A141"/>
+    <mergeCell ref="C139:C141"/>
+    <mergeCell ref="D139:D141"/>
+    <mergeCell ref="A143:A145"/>
+    <mergeCell ref="B143:B145"/>
+    <mergeCell ref="C143:C145"/>
+    <mergeCell ref="D143:D145"/>
+    <mergeCell ref="A147:A149"/>
+    <mergeCell ref="B147:B149"/>
+    <mergeCell ref="C147:C149"/>
+    <mergeCell ref="D147:D149"/>
+    <mergeCell ref="A127:A129"/>
+    <mergeCell ref="B127:B129"/>
+    <mergeCell ref="C127:C129"/>
+    <mergeCell ref="D127:D129"/>
+    <mergeCell ref="C131:C133"/>
+    <mergeCell ref="B131:B133"/>
+    <mergeCell ref="A131:A133"/>
+    <mergeCell ref="D131:D133"/>
+    <mergeCell ref="A135:A137"/>
+    <mergeCell ref="B135:B137"/>
+    <mergeCell ref="C135:C137"/>
+    <mergeCell ref="D135:D137"/>
+    <mergeCell ref="A115:A117"/>
+    <mergeCell ref="B115:B117"/>
+    <mergeCell ref="C115:C117"/>
+    <mergeCell ref="D115:D117"/>
+    <mergeCell ref="A119:A121"/>
+    <mergeCell ref="B119:B121"/>
+    <mergeCell ref="C119:C121"/>
+    <mergeCell ref="D119:D121"/>
+    <mergeCell ref="A123:A125"/>
+    <mergeCell ref="B123:B125"/>
+    <mergeCell ref="C123:C125"/>
+    <mergeCell ref="D123:D125"/>
+    <mergeCell ref="A105:A108"/>
+    <mergeCell ref="B105:B108"/>
+    <mergeCell ref="C105:C108"/>
+    <mergeCell ref="D105:D108"/>
+    <mergeCell ref="E107:E108"/>
+    <mergeCell ref="A110:A113"/>
+    <mergeCell ref="B110:B113"/>
+    <mergeCell ref="C110:C113"/>
+    <mergeCell ref="D110:D113"/>
+    <mergeCell ref="E112:E113"/>
+    <mergeCell ref="A95:A98"/>
+    <mergeCell ref="B95:B98"/>
+    <mergeCell ref="C95:C98"/>
+    <mergeCell ref="D95:D98"/>
+    <mergeCell ref="E97:E98"/>
+    <mergeCell ref="A100:A103"/>
+    <mergeCell ref="B100:B103"/>
+    <mergeCell ref="C100:C103"/>
+    <mergeCell ref="D100:D103"/>
+    <mergeCell ref="E102:E103"/>
+    <mergeCell ref="A86:A88"/>
+    <mergeCell ref="B86:B88"/>
+    <mergeCell ref="C86:C88"/>
+    <mergeCell ref="D86:D88"/>
+    <mergeCell ref="A90:A93"/>
+    <mergeCell ref="B90:B93"/>
+    <mergeCell ref="C90:C93"/>
+    <mergeCell ref="D90:D93"/>
+    <mergeCell ref="E92:E93"/>
+    <mergeCell ref="A74:A76"/>
+    <mergeCell ref="B74:B76"/>
+    <mergeCell ref="C74:C76"/>
+    <mergeCell ref="D74:D76"/>
+    <mergeCell ref="A78:A80"/>
+    <mergeCell ref="B78:B80"/>
+    <mergeCell ref="C78:C80"/>
+    <mergeCell ref="D78:D80"/>
+    <mergeCell ref="A82:A84"/>
+    <mergeCell ref="B82:B84"/>
+    <mergeCell ref="C82:C84"/>
+    <mergeCell ref="D82:D84"/>
+    <mergeCell ref="G127:G129"/>
+    <mergeCell ref="G131:G133"/>
+    <mergeCell ref="G135:G137"/>
+    <mergeCell ref="G139:G141"/>
+    <mergeCell ref="G143:G145"/>
+    <mergeCell ref="G147:G149"/>
+    <mergeCell ref="G151:G153"/>
+    <mergeCell ref="G155:G157"/>
+    <mergeCell ref="G159:G161"/>
     <mergeCell ref="A57:A59"/>
     <mergeCell ref="B57:B59"/>
     <mergeCell ref="C57:C59"/>
     <mergeCell ref="D57:D59"/>
+    <mergeCell ref="A70:A72"/>
+    <mergeCell ref="B70:B72"/>
+    <mergeCell ref="C70:C72"/>
+    <mergeCell ref="D70:D72"/>
+    <mergeCell ref="B61:B64"/>
+    <mergeCell ref="A61:A64"/>
+    <mergeCell ref="C61:C64"/>
+    <mergeCell ref="D61:D64"/>
+    <mergeCell ref="A66:A68"/>
+    <mergeCell ref="B66:B68"/>
+    <mergeCell ref="C66:C68"/>
+    <mergeCell ref="D66:D68"/>
     <mergeCell ref="A47:A49"/>
     <mergeCell ref="B47:B49"/>
     <mergeCell ref="C47:C49"/>
@@ -1695,6 +3164,11 @@
     <mergeCell ref="B51:B52"/>
     <mergeCell ref="C51:C52"/>
     <mergeCell ref="D51:D52"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="C31:C33"/>
     <mergeCell ref="A39:A41"/>
     <mergeCell ref="B39:B41"/>
     <mergeCell ref="C39:C41"/>
@@ -1703,6 +3177,19 @@
     <mergeCell ref="B43:B45"/>
     <mergeCell ref="C43:C45"/>
     <mergeCell ref="D43:D45"/>
+    <mergeCell ref="G54:G55"/>
+    <mergeCell ref="G57:G59"/>
+    <mergeCell ref="G61:G64"/>
+    <mergeCell ref="G66:G68"/>
+    <mergeCell ref="G70:G72"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
     <mergeCell ref="D31:D33"/>
     <mergeCell ref="D28:D29"/>
     <mergeCell ref="A35:A37"/>
@@ -1714,20 +3201,6 @@
     <mergeCell ref="C28:C29"/>
     <mergeCell ref="A31:A33"/>
     <mergeCell ref="B31:B33"/>
-    <mergeCell ref="C31:C33"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="G54:G55"/>
-    <mergeCell ref="G57:G59"/>
-    <mergeCell ref="G61:G63"/>
-    <mergeCell ref="G65:G66"/>
-    <mergeCell ref="G68:G69"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="F11:F13"/>
     <mergeCell ref="G11:G14"/>
@@ -1744,6 +3217,11 @@
     <mergeCell ref="D11:D14"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="B16:B17"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="C8:C9"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="C5:C6"/>
@@ -1751,11 +3229,6 @@
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="B8:B9"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="C8:C9"/>
     <mergeCell ref="G43:G45"/>
     <mergeCell ref="G47:G49"/>
     <mergeCell ref="G51:G52"/>
@@ -1765,8 +3238,21 @@
     <mergeCell ref="G31:G33"/>
     <mergeCell ref="G35:G37"/>
     <mergeCell ref="G39:G41"/>
+    <mergeCell ref="G119:G121"/>
+    <mergeCell ref="G123:G125"/>
+    <mergeCell ref="G95:G98"/>
+    <mergeCell ref="G100:G103"/>
+    <mergeCell ref="G105:G108"/>
+    <mergeCell ref="G110:G113"/>
+    <mergeCell ref="G115:G117"/>
+    <mergeCell ref="G74:G76"/>
+    <mergeCell ref="G78:G80"/>
+    <mergeCell ref="G82:G84"/>
+    <mergeCell ref="G86:G88"/>
+    <mergeCell ref="G90:G93"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>